<commit_message>
Updated Timeplan & Trying new Enemy
</commit_message>
<xml_diff>
--- a/Armpra/Timeplan.xlsx
+++ b/Armpra/Timeplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\armpra\Armpra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC180FBA-A4F3-4035-879F-823293D4B571}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B816D868-72A1-41F7-8B26-5D4991303268}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{5BAF9660-1AAD-4E79-AA8B-F2C71C44E621}"/>
+    <workbookView xWindow="7023" yWindow="1467" windowWidth="26083" windowHeight="13925" xr2:uid="{5BAF9660-1AAD-4E79-AA8B-F2C71C44E621}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Feature Name</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Settings Menu</t>
   </si>
   <si>
-    <t>Textures</t>
-  </si>
-  <si>
     <t>Stelios</t>
   </si>
   <si>
@@ -126,6 +123,24 @@
   </si>
   <si>
     <t>In App Purchases</t>
+  </si>
+  <si>
+    <t>Saving and Loading Progress</t>
+  </si>
+  <si>
+    <t>Particle System</t>
+  </si>
+  <si>
+    <t>Smoother Gameplay</t>
+  </si>
+  <si>
+    <t>PowerUps &amp; Abilities</t>
+  </si>
+  <si>
+    <t>Unlockable Skins</t>
+  </si>
+  <si>
+    <t>More Textures</t>
   </si>
 </sst>
 </file>
@@ -729,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5375F148-E983-438C-8BD6-55F90DCCDEE1}">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -747,7 +762,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="58.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -767,19 +782,19 @@
     </row>
     <row r="2" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="5" t="b">
         <v>1</v>
@@ -791,13 +806,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>1</v>
@@ -809,13 +824,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>1</v>
@@ -827,13 +842,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>1</v>
@@ -845,13 +860,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>1</v>
@@ -863,13 +878,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="7" t="b">
         <v>1</v>
@@ -877,10 +892,10 @@
     </row>
     <row r="8" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4">
         <v>3</v>
@@ -889,7 +904,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="5" t="b">
         <v>0</v>
@@ -898,7 +913,7 @@
     <row r="9" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
@@ -907,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
@@ -925,97 +940,97 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="6">
+    <row r="11" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2">
         <v>3</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="F11" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6">
+        <v>3</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="4">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="4">
         <v>3</v>
       </c>
-      <c r="F13" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="6">
-        <v>2</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="4">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3" t="b">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="9" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="3" t="b">
         <v>0</v>
@@ -1024,34 +1039,89 @@
     <row r="18" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="2">
         <v>1</v>
       </c>
-      <c r="F18" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="6">
-        <v>2</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F23" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="6">
+        <v>3</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="25" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1120,19 +1190,24 @@
     <row r="90" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="91" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="92" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A24"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2:F62">
+  <conditionalFormatting sqref="F2:F67">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C19">
+  <conditionalFormatting sqref="C2:C24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -1142,7 +1217,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F19">
+  <conditionalFormatting sqref="F2:F24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed Acceleration & Updated Timeplan
</commit_message>
<xml_diff>
--- a/Armpra/Timeplan.xlsx
+++ b/Armpra/Timeplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\armpra\Armpra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B816D868-72A1-41F7-8B26-5D4991303268}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEBEBD2-2A57-42CE-A196-AC2E6E5AF320}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7023" yWindow="1467" windowWidth="26083" windowHeight="13925" xr2:uid="{5BAF9660-1AAD-4E79-AA8B-F2C71C44E621}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{5BAF9660-1AAD-4E79-AA8B-F2C71C44E621}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>Feature Name</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>More Textures</t>
+  </si>
+  <si>
+    <t>Score System</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8585"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -744,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5375F148-E983-438C-8BD6-55F90DCCDEE1}">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -901,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>16</v>
@@ -919,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
@@ -931,139 +958,180 @@
     <row r="10" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="9" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
         <v>5</v>
       </c>
-      <c r="F10" s="3" t="b">
-        <v>0</v>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="9" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
       </c>
       <c r="F11" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C13" s="6">
         <v>3</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7" t="b">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="14" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>4</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5" t="b">
+      <c r="D14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2">
+    <row r="16" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6">
         <v>3</v>
       </c>
-      <c r="F14" s="3" t="b">
+      <c r="E16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+    <row r="17" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C17" s="4">
         <v>3</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="2">
-        <v>2</v>
-      </c>
-      <c r="F17" s="3" t="b">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="9" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -1075,7 +1143,7 @@
     <row r="21" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -1087,10 +1155,10 @@
     <row r="22" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3" t="b">
         <v>0</v>
@@ -1099,30 +1167,47 @@
     <row r="23" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3" t="b">
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="10" t="s">
+    <row r="25" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C25" s="6">
         <v>3</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7" t="b">
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1195,20 +1280,21 @@
     <row r="95" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="96" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="97" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A25"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2:F67">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="F2:F68">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C24">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C2:C25">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="5"/>
@@ -1217,9 +1303,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F24">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2:F25">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Visual Changes & More (Still Some Bugs Need Fixes)
- Redesigned Player, Enemies and Bullets to stay consistent with the rounded design language
- Tweaked Player Firepoints
- Completely Rewritten PlayerGeneration Script
</commit_message>
<xml_diff>
--- a/Armpra/Timeplan.xlsx
+++ b/Armpra/Timeplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\armpra\Armpra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9123410A-0F6C-45A8-9994-62AD897BF725}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B65F03-FC76-47A0-9396-6B019FBF23A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{5BAF9660-1AAD-4E79-AA8B-F2C71C44E621}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>Sounds</t>
   </si>
   <si>
-    <t>Advertizing</t>
-  </si>
-  <si>
     <t>Random Level Generation</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>Optimization Updates</t>
+  </si>
+  <si>
+    <t>Advertising</t>
   </si>
 </sst>
 </file>
@@ -763,7 +763,7 @@
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -882,7 +882,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>1</v>
@@ -911,7 +911,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>17</v>
@@ -929,7 +929,7 @@
     <row r="9" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
@@ -947,7 +947,7 @@
     <row r="10" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
@@ -983,7 +983,7 @@
     <row r="12" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>17</v>
@@ -992,7 +992,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>1</v>
@@ -1074,10 +1074,10 @@
     </row>
     <row r="17" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2">
         <v>4</v>
@@ -1089,13 +1089,13 @@
         <v>16</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2">
         <v>4</v>
@@ -1107,13 +1107,13 @@
         <v>16</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -1137,7 +1137,7 @@
     <row r="21" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2">
         <v>3</v>
@@ -1155,7 +1155,7 @@
     <row r="22" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="9" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -1167,7 +1167,7 @@
     <row r="23" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
@@ -1185,7 +1185,7 @@
     <row r="24" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2">
         <v>2</v>
@@ -1194,16 +1194,16 @@
         <v>17</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -1215,7 +1215,7 @@
     <row r="26" spans="1:6" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
       <c r="B26" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>17</v>

</xml_diff>